<commit_message>
modified excel document file
</commit_message>
<xml_diff>
--- a/VINAYTECH_BUSINESS_PAYMENT_DETAILS_DATAMODEL_DATASET.xlsx
+++ b/VINAYTECH_BUSINESS_PAYMENT_DETAILS_DATAMODEL_DATASET.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\Downloads\harshini_business-datamart-test\harshini_business-datamart-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524D8315-4DCA-4788-AEFD-A51A6F17E3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB652981-7851-4AD2-9357-D549EB78F4B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3260" yWindow="2810" windowWidth="14400" windowHeight="7270" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DimStudent" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -7478,10 +7477,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7623,6 +7622,11 @@
       </c>
       <c r="E8">
         <v>1006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>